<commit_message>
add pandas and openpyxl
</commit_message>
<xml_diff>
--- a/data/banco.xlsx
+++ b/data/banco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hurfrais\meu_projeto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935A25C0-778C-478A-930D-F3682CEAE9EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B4BF7C-4FC9-4A95-B157-A541BFA1139C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="75">
   <si>
-    <t>Motor de Tração</t>
-  </si>
-  <si>
     <t>VF120-2018</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>discontinued</t>
   </si>
   <si>
-    <t>Atlas Schindler</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
@@ -245,6 +239,12 @@
   </si>
   <si>
     <t>obsolete</t>
+  </si>
+  <si>
+    <t>Teste banco de dados</t>
+  </si>
+  <si>
+    <t>teste banco de dados</t>
   </si>
 </sst>
 </file>
@@ -655,7 +655,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -670,376 +670,376 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>
-    <ignoredError sqref="A16 A2 D2:E2 A3 C3:E3 A4 C4:E4 A5 C5:E5 A6 C6:E6 A7 C7:E7 A8 C8:E8 A9 C9:E9 A10 C10:E10 A11 C11:E11 A12 C12:E12 A13 C13:E13 A14 C14:E14 A15 C15:E15 C16:E16" numberStoredAsText="1"/>
+    <ignoredError sqref="A16 D2:E2 A3 C3:E3 A4 C4:E4 A5 C5:E5 A6 C6:E6 A7 C7:E7 A8 C8:E8 A9 C9:E9 A10 C10:E10 A11 C11:E11 A12 C12:E12 A13 C13:E13 A14 C14:E14 A15 C15:E15 C16:E16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>